<commit_message>
Start to change the workflow to parallel processing mode similar to Rank score in LPPtiger. Function only till XIC extraction. Rename of multiple lib files. Remove old code.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/FA_Whitelist.xlsx
+++ b/ConfigurationFiles/FA_Whitelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D18"/>
+      <selection activeCell="G13" sqref="G13:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,9 +651,6 @@
       <c r="F13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -665,9 +662,6 @@
       <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -679,9 +673,6 @@
       <c r="F15" t="s">
         <v>20</v>
       </c>
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -693,11 +684,8 @@
       <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -707,11 +695,8 @@
       <c r="F17" t="s">
         <v>20</v>
       </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -719,9 +704,6 @@
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add summary tables to output image with highlight colors. GUI update: save cfg now functional.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/FA_Whitelist.xlsx
+++ b/ConfigurationFiles/FA_Whitelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:G18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +509,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
py2topy3 Remove all the possible conflicts between the TG branch and py2to3
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/FA_Whitelist.xlsx
+++ b/ConfigurationFiles/FA_Whitelist.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>TG</t>
+  </si>
+  <si>
+    <t>FA12:0</t>
+  </si>
+  <si>
+    <t>FA16:1</t>
   </si>
 </sst>
 </file>
@@ -411,18 +417,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,268 +451,302 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>